<commit_message>
a bunch of new figures for 100 meters
</commit_message>
<xml_diff>
--- a/womens_world_records.xlsx
+++ b/womens_world_records.xlsx
@@ -1,13 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunk/Github/Athletics/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC23FB6C-B254-D640-BF38-E0FD060D66F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -626,14 +645,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -644,7 +670,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -661,22 +687,335 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +1035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -709,17 +1048,17 @@
       <c r="D2" t="s">
         <v>148</v>
       </c>
-      <c r="E2" t="n" s="2">
-        <v>21905.0</v>
+      <c r="E2" s="1">
+        <v>21905</v>
       </c>
       <c r="F2" t="s">
         <v>187</v>
       </c>
-      <c r="G2" t="n" s="2">
-        <v>32340.0</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="G2" s="1">
+        <v>32340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -732,17 +1071,17 @@
       <c r="D3" t="s">
         <v>148</v>
       </c>
-      <c r="E3" t="n" s="2">
-        <v>21905.0</v>
+      <c r="E3" s="1">
+        <v>21905</v>
       </c>
       <c r="F3" t="s">
         <v>187</v>
       </c>
-      <c r="G3" t="n" s="2">
-        <v>32415.0</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="1">
+        <v>32415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -755,316 +1094,407 @@
       <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="E4" t="n" s="2">
-        <v>20869.0</v>
+      <c r="E4" s="1">
+        <v>20869</v>
       </c>
       <c r="F4" t="s">
         <v>188</v>
       </c>
-      <c r="G4" t="n" s="2">
-        <v>31326.0</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="G4" s="1">
+        <v>31326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
-        <v>102</v>
+      <c r="C5" s="2">
+        <v>113.28</v>
       </c>
       <c r="D5" t="s">
         <v>150</v>
       </c>
-      <c r="E5" t="n" s="2">
-        <v>18654.0</v>
+      <c r="E5" s="1">
+        <v>18654</v>
       </c>
       <c r="F5" t="s">
         <v>189</v>
       </c>
-      <c r="G5" t="n" s="2">
-        <v>30523.0</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="G5" s="1">
+        <v>30523</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5">
+        <f>H5*86400</f>
+        <v>113.27999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
+      <c r="C6" s="2">
+        <v>148.97999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>151</v>
       </c>
-      <c r="E6" t="n" s="2">
-        <v>24854.0</v>
+      <c r="E6" s="1">
+        <v>24854</v>
       </c>
       <c r="F6" t="s">
         <v>190</v>
       </c>
-      <c r="G6" t="n" s="2">
-        <v>35300.0</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="G6" s="1">
+        <v>35300</v>
+      </c>
+      <c r="H6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I36" si="0">H6*86400</f>
+        <v>148.97999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>104</v>
+      <c r="C7" s="2">
+        <v>230.07</v>
       </c>
       <c r="D7" t="s">
         <v>152</v>
       </c>
-      <c r="E7" t="n" s="2">
-        <v>33277.0</v>
+      <c r="E7" s="1">
+        <v>33277</v>
       </c>
       <c r="F7" t="s">
         <v>191</v>
       </c>
-      <c r="G7" t="n" s="2">
-        <v>42202.0</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="G7" s="1">
+        <v>42202</v>
+      </c>
+      <c r="H7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>230.07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
-        <v>105</v>
+      <c r="C8" s="2">
+        <v>252.33</v>
       </c>
       <c r="D8" t="s">
         <v>153</v>
       </c>
-      <c r="E8" t="n" s="2">
-        <v>33970.0</v>
+      <c r="E8" s="1">
+        <v>33970</v>
       </c>
       <c r="F8" t="s">
         <v>192</v>
       </c>
-      <c r="G8" t="n" s="2">
-        <v>43658.0</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="G8" s="1">
+        <v>43658</v>
+      </c>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>252.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" t="s">
-        <v>106</v>
+      <c r="C9" s="2">
+        <v>323.75</v>
       </c>
       <c r="D9" t="s">
         <v>152</v>
       </c>
-      <c r="E9" t="n" s="2">
-        <v>33277.0</v>
+      <c r="E9" s="1">
+        <v>33277</v>
       </c>
       <c r="F9" t="s">
         <v>191</v>
       </c>
-      <c r="G9" t="n" s="2">
-        <v>42773.0</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="G9" s="1">
+        <v>42773</v>
+      </c>
+      <c r="H9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>323.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
-        <v>107</v>
+      <c r="C10" s="2">
+        <v>486.11</v>
       </c>
       <c r="D10" t="s">
         <v>154</v>
       </c>
-      <c r="E10" t="n" s="2">
-        <v>26673.0</v>
+      <c r="E10" s="1">
+        <v>26673</v>
       </c>
       <c r="F10" t="s">
         <v>193</v>
       </c>
-      <c r="G10" t="n" s="2">
-        <v>34225.0</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="G10" s="1">
+        <v>34225</v>
+      </c>
+      <c r="H10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>486.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" t="s">
-        <v>108</v>
+      <c r="C11" s="2">
+        <v>846.62</v>
       </c>
       <c r="D11" t="s">
         <v>155</v>
       </c>
-      <c r="E11" t="n" s="2">
-        <v>35874.0</v>
+      <c r="E11" s="1">
+        <v>35874</v>
       </c>
       <c r="F11" t="s">
         <v>191</v>
       </c>
-      <c r="G11" t="n" s="2">
-        <v>44111.0</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="G11" s="1">
+        <v>44111</v>
+      </c>
+      <c r="H11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>846.62000000000012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>109</v>
+      <c r="C12" s="2">
+        <v>53280</v>
       </c>
       <c r="D12" t="s">
         <v>156</v>
       </c>
-      <c r="E12" t="n" s="2">
-        <v>34480.0</v>
+      <c r="E12" s="1">
+        <v>34480</v>
       </c>
       <c r="F12" t="s">
         <v>194</v>
       </c>
-      <c r="G12" t="n" s="2">
-        <v>43351.0</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="G12" s="1">
+        <v>43351</v>
+      </c>
+      <c r="H12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>53280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" t="s">
-        <v>110</v>
+      <c r="C13" s="2">
+        <v>53040</v>
       </c>
       <c r="D13" t="s">
         <v>153</v>
       </c>
-      <c r="E13" t="n" s="2">
-        <v>33970.0</v>
+      <c r="E13" s="1">
+        <v>33970</v>
       </c>
       <c r="F13" t="s">
         <v>192</v>
       </c>
-      <c r="G13" t="n" s="2">
-        <v>43513.0</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="G13" s="1">
+        <v>43513</v>
+      </c>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>53039.999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s">
-        <v>111</v>
+      <c r="C14" s="2">
+        <v>1757.45</v>
       </c>
       <c r="D14" t="s">
         <v>157</v>
       </c>
-      <c r="E14" t="n" s="2">
-        <v>33563.0</v>
+      <c r="E14" s="1">
+        <v>33563</v>
       </c>
       <c r="F14" t="s">
         <v>191</v>
       </c>
-      <c r="G14" t="n" s="2">
-        <v>42594.0</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="G14" s="1">
+        <v>42594</v>
+      </c>
+      <c r="H14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>1757.4499999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="C15" t="s">
-        <v>112</v>
+      <c r="C15" s="2">
+        <v>109740</v>
       </c>
       <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="E15" t="n" s="2">
-        <v>28002.0</v>
+      <c r="E15" s="1">
+        <v>28002</v>
       </c>
       <c r="F15" t="s">
         <v>195</v>
       </c>
-      <c r="G15" t="n" s="2">
-        <v>37415.0</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="G15" s="1">
+        <v>37415</v>
+      </c>
+      <c r="H15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>109740</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
-        <v>113</v>
+      <c r="C16" s="2">
+        <v>106980</v>
       </c>
       <c r="D16" t="s">
         <v>159</v>
       </c>
-      <c r="E16" t="n" s="2">
-        <v>34311.0</v>
+      <c r="E16" s="1">
+        <v>34311</v>
       </c>
       <c r="F16" t="s">
         <v>194</v>
       </c>
-      <c r="G16" t="n" s="2">
-        <v>42987.0</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="G16" s="1">
+        <v>42987</v>
+      </c>
+      <c r="H16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>106980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
-        <v>114</v>
+      <c r="C17" s="2">
+        <v>3926.6</v>
       </c>
       <c r="D17" t="s">
         <v>160</v>
       </c>
-      <c r="E17" t="n" s="2">
-        <v>26793.0</v>
+      <c r="E17" s="1">
+        <v>26793</v>
       </c>
       <c r="F17" t="s">
         <v>194</v>
       </c>
-      <c r="G17" t="n" s="2">
-        <v>36772.0</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="G17" s="1">
+        <v>36772</v>
+      </c>
+      <c r="H17" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>3926.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1077,224 +1507,294 @@
       <c r="D18" t="s">
         <v>153</v>
       </c>
-      <c r="E18" t="n" s="2">
-        <v>33970.0</v>
+      <c r="E18" s="1">
+        <v>33970</v>
       </c>
       <c r="F18" t="s">
         <v>192</v>
       </c>
-      <c r="G18" t="n" s="2">
-        <v>44078.0</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="G18" s="1">
+        <v>44078</v>
+      </c>
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>3934.0000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
       </c>
-      <c r="C19" t="s">
-        <v>116</v>
+      <c r="C19" s="2">
+        <v>3934</v>
       </c>
       <c r="D19" t="s">
         <v>161</v>
       </c>
-      <c r="E19" t="n" s="2">
-        <v>34239.0</v>
+      <c r="E19" s="1">
+        <v>34239</v>
       </c>
       <c r="F19" t="s">
         <v>194</v>
       </c>
-      <c r="G19" t="n" s="2">
-        <v>44079.0</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="G19" s="1">
+        <v>44079</v>
+      </c>
+      <c r="H19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
-        <v>117</v>
+      <c r="C20" s="2">
+        <v>3916</v>
       </c>
       <c r="D20" t="s">
         <v>161</v>
       </c>
-      <c r="E20" t="n" s="2">
-        <v>34239.0</v>
+      <c r="E20" s="1">
+        <v>34239</v>
       </c>
       <c r="F20" t="s">
         <v>194</v>
       </c>
-      <c r="G20" t="n" s="2">
-        <v>44121.0</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="G20" s="1">
+        <v>44121</v>
+      </c>
+      <c r="H20" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>3871</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
-        <v>118</v>
+      <c r="C21" s="2">
+        <v>3871</v>
       </c>
       <c r="D21" t="s">
         <v>162</v>
       </c>
-      <c r="E21" t="n" s="2">
-        <v>33441.0</v>
+      <c r="E21" s="1">
+        <v>33441</v>
       </c>
       <c r="F21" t="s">
         <v>191</v>
       </c>
-      <c r="G21" t="n" s="2">
-        <v>43882.0</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="G21" s="1">
+        <v>43882</v>
+      </c>
+      <c r="H21" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>5225.9000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>71</v>
       </c>
-      <c r="C22" t="s">
-        <v>119</v>
+      <c r="C22" s="2">
+        <v>5225.8999999999996</v>
       </c>
       <c r="D22" t="s">
         <v>160</v>
       </c>
-      <c r="E22" t="n" s="2">
-        <v>26793.0</v>
+      <c r="E22" s="1">
+        <v>26793</v>
       </c>
       <c r="F22" t="s">
         <v>194</v>
       </c>
-      <c r="G22" t="n" s="2">
-        <v>37520.0</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="G22" s="1">
+        <v>37520</v>
+      </c>
+      <c r="H22" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>6349.9999999999991</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
+      <c r="C23" s="2">
+        <v>6350</v>
       </c>
       <c r="D23" t="s">
         <v>160</v>
       </c>
-      <c r="E23" t="n" s="2">
-        <v>26793.0</v>
+      <c r="E23" s="1">
+        <v>26793</v>
       </c>
       <c r="F23" t="s">
         <v>194</v>
       </c>
-      <c r="G23" t="n" s="2">
-        <v>37778.0</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="G23" s="1">
+        <v>37778</v>
+      </c>
+      <c r="H23" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>8221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
-        <v>121</v>
+      <c r="C24" s="2">
+        <v>8221</v>
       </c>
       <c r="D24" t="s">
         <v>163</v>
       </c>
-      <c r="E24" t="n" s="2">
-        <v>29969.0</v>
+      <c r="E24" s="1">
+        <v>29969</v>
       </c>
       <c r="F24" t="s">
         <v>194</v>
       </c>
-      <c r="G24" t="n" s="2">
-        <v>42848.0</v>
-      </c>
-    </row>
-    <row r="25">
+      <c r="G24" s="1">
+        <v>42848</v>
+      </c>
+      <c r="H24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>8043.9999999999991</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
-        <v>122</v>
+      <c r="C25" s="2">
+        <v>8044</v>
       </c>
       <c r="D25" t="s">
         <v>164</v>
       </c>
-      <c r="E25" t="n" s="2">
-        <v>34385.0</v>
+      <c r="E25" s="1">
+        <v>34385</v>
       </c>
       <c r="F25" t="s">
         <v>194</v>
       </c>
-      <c r="G25" t="n" s="2">
-        <v>43751.0</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="G25" s="1">
+        <v>43751</v>
+      </c>
+      <c r="H25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>23591.000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="s">
-        <v>123</v>
+      <c r="C26" s="2">
+        <v>23591</v>
       </c>
       <c r="D26" t="s">
         <v>165</v>
       </c>
-      <c r="E26" t="n" s="2">
-        <v>26158.0</v>
+      <c r="E26" s="1">
+        <v>26158</v>
       </c>
       <c r="F26" t="s">
         <v>196</v>
       </c>
-      <c r="G26" t="n" s="2">
-        <v>36702.0</v>
-      </c>
-    </row>
-    <row r="27">
+      <c r="G26" s="1">
+        <v>36702</v>
+      </c>
+      <c r="H26" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>524.31999999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="C27" t="s">
-        <v>124</v>
+      <c r="C27" s="2">
+        <v>524.32000000000005</v>
       </c>
       <c r="D27" t="s">
         <v>166</v>
       </c>
-      <c r="E27" t="n" s="2">
-        <v>33425.0</v>
+      <c r="E27" s="1">
+        <v>33425</v>
       </c>
       <c r="F27" t="s">
         <v>194</v>
       </c>
-      <c r="G27" t="n" s="2">
-        <v>43301.0</v>
-      </c>
-    </row>
-    <row r="28">
+      <c r="G27" s="1">
+        <v>43301</v>
+      </c>
+      <c r="H27" t="s">
+        <v>137</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>2516.23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1307,17 +1807,24 @@
       <c r="D28" t="s">
         <v>167</v>
       </c>
-      <c r="E28" t="n" s="2">
-        <v>33865.0</v>
+      <c r="E28" s="1">
+        <v>33865</v>
       </c>
       <c r="F28" t="s">
         <v>187</v>
       </c>
-      <c r="G28" t="n" s="2">
-        <v>42573.0</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="G28" s="1">
+        <v>42573</v>
+      </c>
+      <c r="H28" t="s">
+        <v>138</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>5212.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1330,17 +1837,24 @@
       <c r="D29" t="s">
         <v>168</v>
       </c>
-      <c r="E29" t="n" s="2">
-        <v>32911.0</v>
+      <c r="E29" s="1">
+        <v>32911</v>
       </c>
       <c r="F29" t="s">
         <v>187</v>
       </c>
-      <c r="G29" t="n" s="2">
-        <v>43742.0</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="G29" s="1">
+        <v>43742</v>
+      </c>
+      <c r="H29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>5078</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1353,17 +1867,24 @@
       <c r="D30" t="s">
         <v>169</v>
       </c>
-      <c r="E30" t="n" s="2">
-        <v>23826.0</v>
+      <c r="E30" s="1">
+        <v>23826</v>
       </c>
       <c r="F30" t="s">
         <v>197</v>
       </c>
-      <c r="G30" t="n" s="2">
-        <v>32019.0</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="G30" s="1">
+        <v>32019</v>
+      </c>
+      <c r="H30" t="s">
+        <v>140</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>14355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1376,17 +1897,24 @@
       <c r="D31" t="s">
         <v>170</v>
       </c>
-      <c r="E31" t="n" s="2">
-        <v>30105.0</v>
+      <c r="E31" s="1">
+        <v>30105</v>
       </c>
       <c r="F31" t="s">
         <v>190</v>
       </c>
-      <c r="G31" t="n" s="2">
-        <v>40053.0</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="G31" s="1">
+        <v>40053</v>
+      </c>
+      <c r="H31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>87.46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1399,17 +1927,24 @@
       <c r="D32" t="s">
         <v>171</v>
       </c>
-      <c r="E32" t="n" s="2">
-        <v>22853.0</v>
+      <c r="E32" s="1">
+        <v>22853</v>
       </c>
       <c r="F32" t="s">
         <v>198</v>
       </c>
-      <c r="G32" t="n" s="2">
-        <v>32305.0</v>
-      </c>
-    </row>
-    <row r="33">
+      <c r="G32" s="1">
+        <v>32305</v>
+      </c>
+      <c r="H32" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>195.17000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1422,17 +1957,24 @@
       <c r="D33" t="s">
         <v>172</v>
       </c>
-      <c r="E33" t="n" s="2">
-        <v>24385.0</v>
+      <c r="E33" s="1">
+        <v>24385</v>
       </c>
       <c r="F33" t="s">
         <v>199</v>
       </c>
-      <c r="G33" t="n" s="2">
-        <v>34921.0</v>
-      </c>
-    </row>
-    <row r="34">
+      <c r="G33" s="1">
+        <v>34921</v>
+      </c>
+      <c r="H33" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>470.17000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1445,17 +1987,24 @@
       <c r="D34" t="s">
         <v>173</v>
       </c>
-      <c r="E34" t="n" s="2">
-        <v>22843.0</v>
+      <c r="E34" s="1">
+        <v>22843</v>
       </c>
       <c r="F34" t="s">
         <v>198</v>
       </c>
-      <c r="G34" t="n" s="2">
-        <v>31935.0</v>
-      </c>
-    </row>
-    <row r="35">
+      <c r="G34" s="1">
+        <v>31935</v>
+      </c>
+      <c r="H34" t="s">
+        <v>145</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>987.01999999999987</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1468,17 +2017,24 @@
       <c r="D35" t="s">
         <v>174</v>
       </c>
-      <c r="E35" t="n" s="2">
-        <v>23277.0</v>
+      <c r="E35" s="1">
+        <v>23277</v>
       </c>
       <c r="F35" t="s">
         <v>188</v>
       </c>
-      <c r="G35" t="n" s="2">
-        <v>32333.0</v>
-      </c>
-    </row>
-    <row r="36">
+      <c r="G35" s="1">
+        <v>32333</v>
+      </c>
+      <c r="H35" t="s">
+        <v>146</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>7901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1491,17 +2047,24 @@
       <c r="D36" t="s">
         <v>175</v>
       </c>
-      <c r="E36" t="n" s="2">
-        <v>31267.0</v>
+      <c r="E36" s="1">
+        <v>31267</v>
       </c>
       <c r="F36" t="s">
         <v>200</v>
       </c>
-      <c r="G36" t="n" s="2">
-        <v>42610.0</v>
-      </c>
-    </row>
-    <row r="37">
+      <c r="G36" s="1">
+        <v>42610</v>
+      </c>
+      <c r="H36" t="s">
+        <v>147</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>636.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1514,17 +2077,17 @@
       <c r="D37" t="s">
         <v>176</v>
       </c>
-      <c r="E37" t="n" s="2">
-        <v>29767.0</v>
+      <c r="E37" s="1">
+        <v>29767</v>
       </c>
       <c r="F37" t="s">
         <v>201</v>
       </c>
-      <c r="G37" t="n" s="2">
-        <v>39704.0</v>
-      </c>
-    </row>
-    <row r="38">
+      <c r="G37" s="1">
+        <v>39704</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1537,17 +2100,17 @@
       <c r="D38" t="s">
         <v>177</v>
       </c>
-      <c r="E38" t="n" s="2">
-        <v>22708.0</v>
+      <c r="E38" s="1">
+        <v>22708</v>
       </c>
       <c r="F38" t="s">
         <v>187</v>
       </c>
-      <c r="G38" t="n" s="2">
-        <v>32410.0</v>
-      </c>
-    </row>
-    <row r="39">
+      <c r="G38" s="1">
+        <v>32410</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1560,109 +2123,109 @@
       <c r="D39" t="s">
         <v>178</v>
       </c>
-      <c r="E39" t="n" s="2">
-        <v>29079.0</v>
+      <c r="E39" s="1">
+        <v>29079</v>
       </c>
       <c r="F39" t="s">
         <v>202</v>
       </c>
-      <c r="G39" t="n" s="2">
-        <v>38457.0</v>
-      </c>
-    </row>
-    <row r="40">
+      <c r="G39" s="1">
+        <v>38457</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C40" t="s">
-        <v>137</v>
+      <c r="C40" s="2">
+        <v>2516.23</v>
       </c>
       <c r="D40" t="s">
         <v>179</v>
       </c>
-      <c r="E40" t="n" s="2">
-        <v>24494.0</v>
+      <c r="E40" s="1">
+        <v>24494</v>
       </c>
       <c r="F40" t="s">
         <v>198</v>
       </c>
-      <c r="G40" t="n" s="2">
-        <v>33078.0</v>
-      </c>
-    </row>
-    <row r="41">
+      <c r="G40" s="1">
+        <v>33078</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>89</v>
       </c>
-      <c r="C41" t="s">
-        <v>138</v>
+      <c r="C41" s="2">
+        <v>5212.3</v>
       </c>
       <c r="D41" t="s">
         <v>180</v>
       </c>
-      <c r="E41" t="n" s="2">
-        <v>25809.0</v>
+      <c r="E41" s="1">
+        <v>25809</v>
       </c>
       <c r="F41" t="s">
         <v>190</v>
       </c>
-      <c r="G41" t="n" s="2">
-        <v>37140.0</v>
-      </c>
-    </row>
-    <row r="42">
+      <c r="G41" s="1">
+        <v>37140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="C42" t="s">
-        <v>139</v>
+      <c r="C42" s="2">
+        <v>5078</v>
       </c>
       <c r="D42" t="s">
         <v>181</v>
       </c>
-      <c r="E42" t="n" s="2">
-        <v>31909.0</v>
+      <c r="E42" s="1">
+        <v>31909</v>
       </c>
       <c r="F42" t="s">
         <v>193</v>
       </c>
-      <c r="G42" t="n" s="2">
-        <v>42161.0</v>
-      </c>
-    </row>
-    <row r="43">
+      <c r="G42" s="1">
+        <v>42161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C43" t="s">
-        <v>140</v>
+      <c r="C43" s="2">
+        <v>14355</v>
       </c>
       <c r="D43" t="s">
         <v>181</v>
       </c>
-      <c r="E43" t="n" s="2">
-        <v>31909.0</v>
+      <c r="E43" s="1">
+        <v>31909</v>
       </c>
       <c r="F43" t="s">
         <v>193</v>
       </c>
-      <c r="G43" t="n" s="2">
-        <v>43533.0</v>
-      </c>
-    </row>
-    <row r="44">
+      <c r="G43" s="1">
+        <v>43533</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1675,155 +2238,155 @@
       <c r="D44" t="s">
         <v>182</v>
       </c>
-      <c r="E44" t="e" s="2">
+      <c r="E44" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F44" t="s">
         <v>187</v>
       </c>
-      <c r="G44" t="n" s="2">
-        <v>41131.0</v>
-      </c>
-    </row>
-    <row r="45">
+      <c r="G44" s="1">
+        <v>41131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
       <c r="B45" t="s">
         <v>93</v>
       </c>
-      <c r="C45" t="s">
-        <v>142</v>
+      <c r="C45" s="2">
+        <v>87.46</v>
       </c>
       <c r="D45" t="s">
         <v>183</v>
       </c>
-      <c r="E45" t="e" s="2">
+      <c r="E45" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F45" t="s">
         <v>187</v>
       </c>
-      <c r="G45" t="n" s="2">
-        <v>36645.0</v>
-      </c>
-    </row>
-    <row r="46">
+      <c r="G45" s="1">
+        <v>36645</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C46" t="s">
-        <v>143</v>
+      <c r="C46" s="2">
+        <v>195.17</v>
       </c>
       <c r="D46" t="s">
         <v>184</v>
       </c>
-      <c r="E46" t="e" s="2">
+      <c r="E46" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F46" t="s">
         <v>198</v>
       </c>
-      <c r="G46" t="n" s="2">
-        <v>32417.0</v>
-      </c>
-    </row>
-    <row r="47">
+      <c r="G46" s="1">
+        <v>32417</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>51</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
       </c>
-      <c r="C47" t="s">
-        <v>144</v>
+      <c r="C47" s="2">
+        <v>470.17</v>
       </c>
       <c r="D47" t="s">
         <v>184</v>
       </c>
-      <c r="E47" t="e" s="2">
+      <c r="E47" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F47" t="s">
         <v>198</v>
       </c>
-      <c r="G47" t="n" s="2">
-        <v>30899.0</v>
-      </c>
-    </row>
-    <row r="48">
+      <c r="G47" s="1">
+        <v>30899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
       <c r="B48" t="s">
         <v>96</v>
       </c>
-      <c r="C48" t="s">
-        <v>145</v>
+      <c r="C48" s="2">
+        <v>987.02</v>
       </c>
       <c r="D48" t="s">
         <v>185</v>
       </c>
-      <c r="E48" t="e" s="2">
+      <c r="E48" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F48" t="s">
         <v>187</v>
       </c>
-      <c r="G48" t="n" s="2">
-        <v>44043.0</v>
-      </c>
-    </row>
-    <row r="49">
+      <c r="G48" s="1">
+        <v>44043</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C49" t="s">
-        <v>146</v>
+      <c r="C49" s="2">
+        <v>7901</v>
       </c>
       <c r="D49" t="s">
         <v>186</v>
       </c>
-      <c r="E49" t="e" s="2">
+      <c r="E49" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F49" t="s">
         <v>193</v>
       </c>
-      <c r="G49" t="n" s="2">
-        <v>35854.0</v>
-      </c>
-    </row>
-    <row r="50">
+      <c r="G49" s="1">
+        <v>35854</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
       <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="C50" t="s">
-        <v>147</v>
+      <c r="C50" s="2">
+        <v>636.5</v>
       </c>
       <c r="D50" t="s">
         <v>182</v>
       </c>
-      <c r="E50" t="e" s="2">
+      <c r="E50" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="F50" t="s">
         <v>187</v>
       </c>
-      <c r="G50" t="n" s="2">
-        <v>42126.0</v>
+      <c r="G50" s="1">
+        <v>42126</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>